<commit_message>
Try to show error to user
</commit_message>
<xml_diff>
--- a/public/files/Comments1_1.xlsx
+++ b/public/files/Comments1_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995"/>
+    <workbookView xWindow="390" yWindow="630" windowWidth="18855" windowHeight="8895"/>
   </bookViews>
   <sheets>
     <sheet name="Excel sheet" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Academic Year</t>
   </si>
@@ -52,6 +52,9 @@
     <t>2600081171</t>
   </si>
   <si>
+    <t>Arissara Wuthisasna</t>
+  </si>
+  <si>
     <t>2600081172</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t>2600081173</t>
   </si>
   <si>
+    <t>Chakree Kenganantanon</t>
+  </si>
+  <si>
     <t>2600081174</t>
   </si>
   <si>
@@ -229,31 +235,10 @@
     <t>Melisa Tunchumrus</t>
   </si>
   <si>
-    <t>test ja</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>teststdsfsdf</t>
-  </si>
-  <si>
-    <t>Arissara Wuthisasnaa</t>
-  </si>
-  <si>
-    <t>werwerwer</t>
-  </si>
-  <si>
-    <t>Chakreesad Kenganantanon</t>
-  </si>
-  <si>
-    <t>fsdf</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>asdasdass</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>tse</t>
   </si>
 </sst>
 </file>
@@ -611,7 +596,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -672,8 +657,8 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>71</v>
+      <c r="C5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>73</v>
@@ -689,269 +674,245 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Show error when upload Comment
</commit_message>
<xml_diff>
--- a/public/files/Comments1_1.xlsx
+++ b/public/files/Comments1_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="18855" windowHeight="8895"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995"/>
   </bookViews>
   <sheets>
     <sheet name="Excel sheet" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Academic Year</t>
   </si>
@@ -55,15 +55,9 @@
     <t>Arissara Wuthisasna</t>
   </si>
   <si>
-    <t>2600081172</t>
-  </si>
-  <si>
     <t>Asawin Srisuphapreeda</t>
   </si>
   <si>
-    <t>2600081173</t>
-  </si>
-  <si>
     <t>Chakree Kenganantanon</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>Grace Tirachulisoonthorn</t>
   </si>
   <si>
-    <t>2600081175</t>
-  </si>
-  <si>
     <t>Jiratthaya Jirarojwong</t>
   </si>
   <si>
@@ -94,18 +85,12 @@
     <t>2600081178</t>
   </si>
   <si>
-    <t>Leartrat Tangvongleart</t>
-  </si>
-  <si>
     <t>2600081179</t>
   </si>
   <si>
     <t>Manutchanika Paitoonrajitpipit</t>
   </si>
   <si>
-    <t>2600081180</t>
-  </si>
-  <si>
     <t>Naphat Thanaphan</t>
   </si>
   <si>
@@ -118,9 +103,6 @@
     <t>2600081182</t>
   </si>
   <si>
-    <t>Natrada Jermnarong</t>
-  </si>
-  <si>
     <t>2600081184</t>
   </si>
   <si>
@@ -235,10 +217,19 @@
     <t>Melisa Tunchumrus</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>tse</t>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Leartrat Tangvonglearta</t>
+  </si>
+  <si>
+    <t>adf</t>
   </si>
 </sst>
 </file>
@@ -596,7 +587,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -657,9 +648,6 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -668,251 +656,254 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
+      <c r="D7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
+      <c r="A15" s="1">
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
importPage can upload multiple files. Now remain validate
</commit_message>
<xml_diff>
--- a/public/files/Comments1_1.xlsx
+++ b/public/files/Comments1_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995"/>
+    <workbookView xWindow="390" yWindow="630" windowWidth="18855" windowHeight="8895"/>
   </bookViews>
   <sheets>
     <sheet name="Excel sheet" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
   <si>
     <t>Academic Year</t>
   </si>
@@ -55,9 +55,15 @@
     <t>Arissara Wuthisasna</t>
   </si>
   <si>
+    <t>2600081172</t>
+  </si>
+  <si>
     <t>Asawin Srisuphapreeda</t>
   </si>
   <si>
+    <t>2600081173</t>
+  </si>
+  <si>
     <t>Chakree Kenganantanon</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
     <t>Grace Tirachulisoonthorn</t>
   </si>
   <si>
+    <t>2600081175</t>
+  </si>
+  <si>
     <t>Jiratthaya Jirarojwong</t>
   </si>
   <si>
@@ -85,12 +94,18 @@
     <t>2600081178</t>
   </si>
   <si>
+    <t>Leartrat Tangvongleart</t>
+  </si>
+  <si>
     <t>2600081179</t>
   </si>
   <si>
     <t>Manutchanika Paitoonrajitpipit</t>
   </si>
   <si>
+    <t>2600081180</t>
+  </si>
+  <si>
     <t>Naphat Thanaphan</t>
   </si>
   <si>
@@ -103,6 +118,9 @@
     <t>2600081182</t>
   </si>
   <si>
+    <t>Natrada Jermnarong</t>
+  </si>
+  <si>
     <t>2600081184</t>
   </si>
   <si>
@@ -217,19 +235,19 @@
     <t>Melisa Tunchumrus</t>
   </si>
   <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>zxcv</t>
+  </si>
+  <si>
     <t>asdf</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>Leartrat Tangvonglearta</t>
-  </si>
-  <si>
-    <t>adf</t>
+    <t>asfd</t>
   </si>
 </sst>
 </file>
@@ -587,7 +605,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -659,251 +677,260 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>123</v>
+      <c r="A15" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>